<commit_message>
New scenarios, data-output integration
There are a couple new scenarios added to the Connors test map, and data output is now being handled as a plugin call.
</commit_message>
<xml_diff>
--- a/Bystander Intervention/MetaData/MetaData.xlsx
+++ b/Bystander Intervention/MetaData/MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Documents\Games\SeniorDesign480\Bystander Intervention\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F22877B-23FE-40D3-9660-3B852F3E9435}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6B2EB1-0288-453E-A8A2-D82D75680024}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7710" yWindow="4665" windowWidth="20910" windowHeight="11835" xr2:uid="{6CCB2488-0D6D-4EC9-A2A8-43151E4FAC94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6CCB2488-0D6D-4EC9-A2A8-43151E4FAC94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Title</t>
   </si>
@@ -405,6 +405,9 @@
     <t xml:space="preserve">Update from you: Well, I could have helped someone\n
 out today. I didn't, and they dropped all of their \n
 things everwhere. </t>
+  </si>
+  <si>
+    <t>BestChoice?</t>
   </si>
 </sst>
 </file>
@@ -759,13 +762,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED39810-76AD-4451-B4B4-55408CB96D54}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,9 +782,10 @@
     <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="150.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -812,8 +816,11 @@
       <c r="J1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -835,8 +842,11 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -858,8 +868,11 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -881,8 +894,11 @@
       <c r="I4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -901,8 +917,11 @@
       <c r="H5" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
@@ -921,8 +940,11 @@
       <c r="H6" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29</v>
       </c>
@@ -941,8 +963,11 @@
       <c r="H7" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -961,8 +986,11 @@
       <c r="H8" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>33</v>
       </c>
@@ -972,8 +1000,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -986,8 +1017,11 @@
       <c r="I10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>42</v>
       </c>
@@ -997,8 +1031,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>47</v>
       </c>
@@ -1008,8 +1045,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>49</v>
       </c>
@@ -1019,8 +1059,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51</v>
       </c>
@@ -1030,8 +1073,11 @@
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>59</v>
       </c>
@@ -1041,8 +1087,11 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>76</v>
       </c>
@@ -1052,8 +1101,11 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>80</v>
       </c>
@@ -1063,8 +1115,11 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>82</v>
       </c>
@@ -1074,8 +1129,11 @@
       <c r="C18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>52</v>
       </c>
@@ -1085,8 +1143,11 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>67</v>
       </c>
@@ -1096,8 +1157,11 @@
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1107,8 +1171,11 @@
       <c r="C21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1118,8 +1185,11 @@
       <c r="C22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1129,8 +1199,11 @@
       <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1140,8 +1213,11 @@
       <c r="C24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1151,8 +1227,11 @@
       <c r="C25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1165,8 +1244,11 @@
       <c r="I26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>31</v>
       </c>
@@ -1176,8 +1258,11 @@
       <c r="C27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>32</v>
       </c>
@@ -1187,8 +1272,11 @@
       <c r="C28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>34</v>
       </c>
@@ -1198,8 +1286,11 @@
       <c r="C29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>35</v>
       </c>
@@ -1209,8 +1300,11 @@
       <c r="C30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43</v>
       </c>
@@ -1220,8 +1314,11 @@
       <c r="C31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>44</v>
       </c>
@@ -1231,8 +1328,11 @@
       <c r="C32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>50</v>
       </c>
@@ -1242,8 +1342,11 @@
       <c r="C33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>53</v>
       </c>
@@ -1253,8 +1356,11 @@
       <c r="C34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>58</v>
       </c>
@@ -1264,8 +1370,11 @@
       <c r="C35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>60</v>
       </c>
@@ -1275,8 +1384,11 @@
       <c r="C36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>73</v>
       </c>
@@ -1286,8 +1398,11 @@
       <c r="C37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>83</v>
       </c>
@@ -1297,8 +1412,11 @@
       <c r="C38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>24</v>
       </c>
@@ -1308,8 +1426,11 @@
       <c r="C39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>65</v>
       </c>
@@ -1319,8 +1440,11 @@
       <c r="C40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1330,8 +1454,11 @@
       <c r="C41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10</v>
       </c>
@@ -1344,8 +1471,11 @@
       <c r="I42" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -1355,8 +1485,11 @@
       <c r="C43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>23</v>
       </c>
@@ -1366,8 +1499,11 @@
       <c r="C44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>37</v>
       </c>
@@ -1377,8 +1513,11 @@
       <c r="C45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41</v>
       </c>
@@ -1388,8 +1527,11 @@
       <c r="C46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>55</v>
       </c>
@@ -1399,8 +1541,11 @@
       <c r="C47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>57</v>
       </c>
@@ -1410,8 +1555,11 @@
       <c r="C48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>61</v>
       </c>
@@ -1421,8 +1569,11 @@
       <c r="C49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>63</v>
       </c>
@@ -1432,8 +1583,11 @@
       <c r="C50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>75</v>
       </c>
@@ -1443,8 +1597,11 @@
       <c r="C51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>46</v>
       </c>
@@ -1454,8 +1611,11 @@
       <c r="C52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>86</v>
       </c>
@@ -1468,8 +1628,11 @@
       <c r="I53" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1482,8 +1645,11 @@
       <c r="I54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1493,8 +1659,11 @@
       <c r="C55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>14</v>
       </c>
@@ -1504,8 +1673,11 @@
       <c r="C56">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>36</v>
       </c>
@@ -1515,8 +1687,11 @@
       <c r="C57">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>39</v>
       </c>
@@ -1526,8 +1701,11 @@
       <c r="C58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>62</v>
       </c>
@@ -1537,8 +1715,11 @@
       <c r="C59">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>64</v>
       </c>
@@ -1548,8 +1729,11 @@
       <c r="C60">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>68</v>
       </c>
@@ -1559,8 +1743,11 @@
       <c r="C61">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>71</v>
       </c>
@@ -1570,8 +1757,11 @@
       <c r="C62">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>78</v>
       </c>
@@ -1581,8 +1771,11 @@
       <c r="C63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>87</v>
       </c>
@@ -1592,8 +1785,11 @@
       <c r="C64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>88</v>
       </c>
@@ -1603,8 +1799,11 @@
       <c r="C65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -1614,8 +1813,11 @@
       <c r="C66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1628,8 +1830,11 @@
       <c r="I67" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>19</v>
       </c>
@@ -1639,8 +1844,11 @@
       <c r="C68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>20</v>
       </c>
@@ -1650,8 +1858,11 @@
       <c r="C69">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>21</v>
       </c>
@@ -1661,8 +1872,11 @@
       <c r="C70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>22</v>
       </c>
@@ -1672,8 +1886,11 @@
       <c r="C71">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>66</v>
       </c>
@@ -1683,8 +1900,11 @@
       <c r="C72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>69</v>
       </c>
@@ -1694,8 +1914,11 @@
       <c r="C73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>70</v>
       </c>
@@ -1705,8 +1928,11 @@
       <c r="C74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -1716,8 +1942,11 @@
       <c r="C75">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>77</v>
       </c>
@@ -1727,8 +1956,11 @@
       <c r="C76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>11</v>
       </c>
@@ -1738,8 +1970,11 @@
       <c r="C77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>84</v>
       </c>
@@ -1749,8 +1984,11 @@
       <c r="C78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>85</v>
       </c>
@@ -1759,6 +1997,9 @@
       </c>
       <c r="C79">
         <v>5</v>
+      </c>
+      <c r="K79">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>